<commit_message>
updated to inline version
</commit_message>
<xml_diff>
--- a/TestObjectHandler.xlsx
+++ b/TestObjectHandler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First</t>
   </si>
@@ -48,13 +48,16 @@
     <t>MyArray.getSum</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>Hello World</t>
-  </si>
-  <si>
     <t>AsyncMySlowFunction</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>wait</t>
   </si>
 </sst>
 </file>
@@ -119,18 +122,18 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.33e8aa176ba544eebc00bc6b91f41d1b">
+    <main first="rtdsrv.267b62acad374e91b656c222cdcacef0">
       <tp t="s">
-        <v>[MyArray.1]</v>
+        <v>[Person.3]</v>
         <stp/>
-        <stp>[MyArray.1]</stp>
-        <tr r="F6" s="1"/>
+        <stp>[Person.3]</stp>
+        <tr r="F3" s="1"/>
       </tp>
       <tp t="s">
-        <v>[Person.1]</v>
+        <v>[MyArray.3]</v>
         <stp/>
-        <stp>[Person.1]</stp>
-        <tr r="F3" s="1"/>
+        <stp>[MyArray.3]</stp>
+        <tr r="F6" s="1"/>
       </tp>
     </main>
   </volType>
@@ -426,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +463,7 @@
       </c>
       <c r="F3" t="str">
         <f>_xll.Person.create(D3,E3)</f>
-        <v>[Person.1]</v>
+        <v>[Person.3]</v>
       </c>
       <c r="G3" t="str">
         <f>_xll.Person.getFirstName(F3)</f>
@@ -490,7 +493,7 @@
       </c>
       <c r="F6" t="str">
         <f>_xll.MyArray.create(D6,E6)</f>
-        <v>[MyArray.1]</v>
+        <v>[MyArray.3]</v>
       </c>
       <c r="G6">
         <f>_xll.MyArray.getSum(F6)</f>
@@ -499,19 +502,25 @@
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>11</v>
       </c>
+      <c r="E9">
+        <v>2000</v>
+      </c>
       <c r="F9" t="str">
-        <f>_xll.AsyncMySlowFunction(D9)</f>
-        <v>Hello World</v>
+        <f>_xll.AsyncMySlowFunction(D9,E9)</f>
+        <v>hello</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ArrayResizer and asyncRunAndResize method
</commit_message>
<xml_diff>
--- a/TestObjectHandler.xlsx
+++ b/TestObjectHandler.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>First</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Hope</t>
   </si>
   <si>
-    <t>Person.getFirstName</t>
-  </si>
-  <si>
     <t>Person.create</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>MyArray.getSum</t>
-  </si>
-  <si>
     <t>AsyncMySlowFunction</t>
   </si>
   <si>
@@ -57,7 +51,37 @@
     <t>message</t>
   </si>
   <si>
-    <t>wait</t>
+    <t>AsyncMyBigSlowFunction</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>columns</t>
+  </si>
+  <si>
+    <t>Example 1 - Object Handler for Class</t>
+  </si>
+  <si>
+    <t>Example 2 - Object Handler for Array</t>
+  </si>
+  <si>
+    <t>creates array from [a .. a+n]</t>
+  </si>
+  <si>
+    <t>Example 3 - Inline Async</t>
+  </si>
+  <si>
+    <t>Example 4 - Inline Async and Resize</t>
+  </si>
+  <si>
+    <t>getFirstName</t>
+  </si>
+  <si>
+    <t>getSum</t>
+  </si>
+  <si>
+    <t>wait(ms)</t>
   </si>
 </sst>
 </file>
@@ -90,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -98,13 +122,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,18 +252,20 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.267b62acad374e91b656c222cdcacef0">
+    <main first="rtdsrv.2a34ed13371c4f68926c6fa79b18a394">
       <tp t="s">
-        <v>[Person.3]</v>
+        <v>[Person.1]</v>
         <stp/>
-        <stp>[Person.3]</stp>
-        <tr r="F3" s="1"/>
+        <stp>[Person.1]</stp>
+        <tr r="G4" s="1"/>
       </tp>
+    </main>
+    <main first="rtdsrv.2a34ed13371c4f68926c6fa79b18a394">
       <tp t="s">
-        <v>[MyArray.3]</v>
+        <v>[MyArray.1]</v>
         <stp/>
-        <stp>[MyArray.3]</stp>
-        <tr r="F6" s="1"/>
+        <stp>[MyArray.1]</stp>
+        <tr r="G10" s="1"/>
       </tp>
     </main>
   </volType>
@@ -427,100 +559,354 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:G9"/>
+  <dimension ref="B1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="14" t="str">
+        <f>_xll.Person.create(C4,D4)</f>
+        <v>[Person.1]</v>
+      </c>
+      <c r="H4" s="14" t="str">
+        <f>_xll.Person.getFirstName(G4)</f>
+        <v>Bob</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H9" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="14">
+        <v>10</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="14" t="str">
+        <f>_xll.MyArray.create(C10,D10)</f>
+        <v>[MyArray.1]</v>
+      </c>
+      <c r="H10" s="14">
+        <f>_xll.MyArray.getSum(G10)</f>
+        <v>55</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2000</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14" t="str">
+        <f>_xll.AsyncMySlowFunction(C16,D16)</f>
+        <v>hello</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="H20">
+        <f t="array" ref="H20:N24">_xll.AsyncResizeMyBigSlowFunction(C21,D21,E21)</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="14">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14">
+        <v>7</v>
+      </c>
+      <c r="E21" s="14">
+        <v>500</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J21">
         <v>3</v>
       </c>
-      <c r="F3" t="str">
-        <f>_xll.Person.create(D3,E3)</f>
-        <v>[Person.3]</v>
-      </c>
-      <c r="G3" t="str">
-        <f>_xll.Person.getFirstName(F3)</f>
-        <v>Bob</v>
-      </c>
-    </row>
-    <row r="5" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="s">
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21">
         <v>7</v>
       </c>
-      <c r="E5" s="1" t="s">
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11"/>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <v>7</v>
+      </c>
+      <c r="N22">
         <v>8</v>
       </c>
-      <c r="F5" s="1" t="s">
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
         <v>6</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="L23">
+        <v>7</v>
+      </c>
+      <c r="M23">
+        <v>8</v>
+      </c>
+      <c r="N23">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>5</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <v>9</v>
+      </c>
+      <c r="N24">
         <v>10</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <f>_xll.MyArray.create(D6,E6)</f>
-        <v>[MyArray.3]</v>
-      </c>
-      <c r="G6">
-        <f>_xll.MyArray.getSum(F6)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>2000</v>
-      </c>
-      <c r="F9" t="str">
-        <f>_xll.AsyncMySlowFunction(D9,E9)</f>
-        <v>hello</v>
       </c>
     </row>
   </sheetData>

</xml_diff>